<commit_message>
commit regarding to operations
</commit_message>
<xml_diff>
--- a/src/assets/Download/temp-container.xlsx
+++ b/src/assets/Download/temp-container.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650"/>
+    <workbookView windowWidth="20490" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>containerNumber</t>
   </si>
   <si>
     <t>containerType</t>
+  </si>
+  <si>
+    <t>isEmpty</t>
   </si>
   <si>
     <t>c100001</t>
@@ -197,7 +200,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,12 +252,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,76 +592,76 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1211,48 +1208,60 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="25.1428571428571" customWidth="1"/>
     <col min="2" max="3" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Misc change in Consignment Entry
</commit_message>
<xml_diff>
--- a/src/assets/Download/temp-container.xlsx
+++ b/src/assets/Download/temp-container.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7200"/>
+    <workbookView windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>containerNumber</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t>20 ft Standard</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
   <si>
     <t>c100003</t>
@@ -1211,7 +1217,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -1238,8 +1244,8 @@
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="b">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1249,19 +1255,19 @@
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="b">
-        <v>0</v>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C4" s="2" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>